<commit_message>
SXSSF formulas support demo (via UpdateCellCommand)
</commit_message>
<xml_diff>
--- a/src/main/resources/org/jxls/demo/sxssf_template.xlsx
+++ b/src/main/resources/org/jxls/demo/sxssf_template.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -27,7 +27,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="238"/>
           </rPr>
           <t>Автор:</t>
         </r>
@@ -36,10 +37,11 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="238"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="D4")</t>
+jx:area(lastCell="E4")</t>
         </r>
       </text>
     </comment>
@@ -51,7 +53,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="238"/>
           </rPr>
           <t>Автор:</t>
         </r>
@@ -60,10 +63,37 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="238"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="employees" var="employee" lastCell="D4")</t>
+jx:each(items="employees" var="employee" lastCell="E4")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>Автор:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:updateCell(lastCell="E4"  updater="totalCellUpdater")</t>
         </r>
       </text>
     </comment>
@@ -72,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -98,7 +128,10 @@
     <t>${employee.bonus}</t>
   </si>
   <si>
-    <t>Object Collection Demo</t>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Simple SXSSF Output</t>
   </si>
 </sst>
 </file>
@@ -106,8 +139,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -121,14 +154,16 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
     <font>
       <b/>
@@ -181,14 +216,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -490,30 +526,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.578125" customWidth="1"/>
-    <col min="2" max="2" width="14.578125" customWidth="1"/>
-    <col min="3" max="3" width="21.26171875" customWidth="1"/>
-    <col min="4" max="4" width="16.83984375" customWidth="1"/>
+    <col min="1" max="1" width="18.59765625" customWidth="1"/>
+    <col min="2" max="2" width="14.59765625" customWidth="1"/>
+    <col min="3" max="3" width="21.265625" customWidth="1"/>
+    <col min="4" max="4" width="16.86328125" customWidth="1"/>
+    <col min="5" max="5" width="13.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A1" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -526,8 +562,11 @@
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -539,6 +578,10 @@
       </c>
       <c r="D4" s="6" t="s">
         <v>7</v>
+      </c>
+      <c r="E4" s="7" t="e">
+        <f>C4*(1+D4)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
complete SXSSF formulas demo
</commit_message>
<xml_diff>
--- a/src/main/resources/org/jxls/demo/sxssf_template.xlsx
+++ b/src/main/resources/org/jxls/demo/sxssf_template.xlsx
@@ -93,7 +93,7 @@
             <charset val="238"/>
           </rPr>
           <t xml:space="preserve">
-jx:updateCell(lastCell="E4"  updater="totalCellUpdater")</t>
+jx:updateCell(lastCell="E4"  updater="cellRefUpdater")</t>
         </r>
       </text>
     </comment>
@@ -216,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -224,7 +224,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -579,7 +578,7 @@
       <c r="D4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="7" t="e">
+      <c r="E4" s="5" t="e">
         <f>C4*(1+D4)</f>
         <v>#VALUE!</v>
       </c>

</xml_diff>